<commit_message>
modified the log processing script
</commit_message>
<xml_diff>
--- a/scripts/drone_app/processLogs/Comparison_template.xlsx
+++ b/scripts/drone_app/processLogs/Comparison_template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasamanamannejad/workspace_all/research/edge-offloading/scripts/drone_app/processLogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasamanamannejad/workspace_all/research/edge-offloading/sim_results/ite1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CCD5EC-60F7-A746-94E9-BEC344C11E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84265A2C-99E5-2F4A-B29B-B4CFABD7852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="26860" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="26860" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL_APP" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ALL_APP!$C$1:$C$2754</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ALL_APP!$C$1:$C$969</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>AI</t>
   </si>
@@ -49,7 +49,16 @@
     <t>Random</t>
   </si>
   <si>
-    <t>total</t>
+    <t>total Completed</t>
+  </si>
+  <si>
+    <t>total failed</t>
+  </si>
+  <si>
+    <t>total uncompleted</t>
+  </si>
+  <si>
+    <t>Total Tasks</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +402,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -554,13 +569,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -919,31 +935,34 @@
   <dimension ref="A1:AB969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="X1" sqref="X1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="4.83203125" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="10.83203125" style="5"/>
+    <col min="4" max="4" width="7.83203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="4.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" customWidth="1"/>
     <col min="9" max="9" width="5.1640625" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="5"/>
+    <col min="10" max="10" width="10.83203125" style="5"/>
+    <col min="11" max="11" width="7.1640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="4.1640625" customWidth="1"/>
-    <col min="14" max="14" width="19.5" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="8.5" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="18" width="10.83203125" style="5"/>
+    <col min="17" max="17" width="10.83203125" style="5"/>
+    <col min="18" max="18" width="8.5" style="5" customWidth="1"/>
     <col min="19" max="19" width="3.83203125" customWidth="1"/>
-    <col min="21" max="21" width="19.5" customWidth="1"/>
+    <col min="21" max="21" width="15.5" customWidth="1"/>
     <col min="22" max="22" width="7.6640625" customWidth="1"/>
     <col min="23" max="23" width="8.1640625" customWidth="1"/>
     <col min="24" max="25" width="10.83203125" style="5"/>
     <col min="26" max="26" width="4" customWidth="1"/>
-    <col min="28" max="28" width="19.5" customWidth="1"/>
+    <col min="28" max="28" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
@@ -958,7 +977,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G1" t="e">
-        <f>F1/G$7*100</f>
+        <f>AVERAGE(G21,G26,G31,G36,G41,G46,G51,G56,G61,G66,G71,G76,G81,G86,G91,G96,G101,G106)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -968,11 +987,11 @@
         <v>100</v>
       </c>
       <c r="M1" t="e">
-        <f t="shared" ref="M1:M32" si="1">AVERAGEIF(J:J,J1,K:K)</f>
+        <f>AVERAGEIF(J:J,J1,K:K)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N1" t="e">
-        <f>M1/N$7*100</f>
+        <f>AVERAGE(N21,N26,N31,N36,N41,N46,N51,N56,N61,N66,N71,N76,N81,N86,N91,N96,N101,N106)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -986,7 +1005,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U1" t="e">
-        <f>T1/U$7*100</f>
+        <f>AVERAGE(U21,U26,U31,U36,U41,U46,U51,U56,U61,U66,U71,U76,U81,U86,U91,U96,U101,U106)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V1" s="3" t="s">
@@ -996,11 +1015,11 @@
         <v>100</v>
       </c>
       <c r="AA1" t="e">
-        <f t="shared" ref="AA1:AA53" si="2">AVERAGEIF(X:X,X1,Y:Y)</f>
+        <f>AVERAGEIF(X:X,X1,Y:Y)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB1" t="e">
-        <f>AA1/AB$7*100</f>
+        <f>AVERAGE(AB21,AB26,AB31,AB36,AB41,AB46,AB51,AB56,AB61,AB66,AB71,AB76,AB81,AB86,AB91,AB96,AB101,AB106)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1013,40 +1032,40 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G2" t="e">
-        <f>F2/G$7*100</f>
+        <f t="shared" ref="G2:G3" si="1">AVERAGE(G22,G27,G32,G37,G42,G47,G52,G57,G62,G67,G72,G77,G82,G87,G92,G97,G102,G107)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I2" s="2">
         <v>100</v>
       </c>
       <c r="M2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="M2:M32" si="2">AVERAGEIF(J:J,J2,K:K)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N2" t="e">
-        <f>M2/N$7*100</f>
+        <f t="shared" ref="N2:N3" si="3">AVERAGE(N22,N27,N32,N37,N42,N47,N52,N57,N62,N67,N72,N77,N82,N87,N92,N97,N102,N107)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P2" s="2">
         <v>100</v>
       </c>
       <c r="T2" t="e">
-        <f t="shared" ref="T1:T53" si="3">AVERAGEIF(Q:Q,Q2,R:R)</f>
+        <f t="shared" ref="T2:T53" si="4">AVERAGEIF(Q:Q,Q2,R:R)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U2" t="e">
-        <f>T2/U$7*100</f>
+        <f t="shared" ref="U2:U3" si="5">AVERAGE(U22,U27,U32,U37,U42,U47,U52,U57,U62,U67,U72,U77,U82,U87,U92,U97,U102,U107)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W2" s="2">
         <v>100</v>
       </c>
       <c r="AA2" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AA2:AA53" si="6">AVERAGEIF(X:X,X2,Y:Y)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB2" t="e">
-        <f>AA2/AB$7*100</f>
+        <f t="shared" ref="AB2:AB3" si="7">AVERAGE(AB22,AB27,AB32,AB37,AB42,AB47,AB52,AB57,AB62,AB67,AB72,AB77,AB82,AB87,AB92,AB97,AB102,AB107)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1059,40 +1078,40 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G3" t="e">
-        <f>F3/G$7*100</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I3" s="2">
         <v>100</v>
       </c>
       <c r="M3" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N3" t="e">
-        <f>M3/N$7*100</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P3" s="2">
         <v>100</v>
       </c>
       <c r="T3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U3" t="e">
-        <f>T3/U$7*100</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W3" s="2">
         <v>100</v>
       </c>
       <c r="AA3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB3" t="e">
-        <f>AA3/AB$7*100</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1108,21 +1127,21 @@
         <v>100</v>
       </c>
       <c r="M4" t="e">
-        <f t="shared" si="1"/>
+        <f>AVERAGEIF(J:J,J4,K:K)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P4" s="2">
         <v>100</v>
       </c>
       <c r="T4" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W4" s="2">
         <v>100</v>
       </c>
       <c r="AA4" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1134,25 +1153,41 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G5" t="e">
+        <f>D1/SUM(D1:D3)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I5" s="2">
         <v>100</v>
       </c>
       <c r="M5" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" t="e">
+        <f>K1/SUM(K1:K3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P5" s="2">
         <v>100</v>
       </c>
       <c r="T5" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U5" t="e">
+        <f>R1/SUM(R1:R3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W5" s="2">
         <v>100</v>
       </c>
       <c r="AA5" t="e">
-        <f>AVERAGEIF(X:X,X5,Y:Y)</f>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB5" t="e">
+        <f>Y1/SUM(Y1:Y3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1164,38 +1199,42 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G6" t="s">
-        <v>4</v>
+      <c r="G6" s="2" t="e">
+        <f>D2/SUM(D1:D3)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="I6" s="2">
         <v>100</v>
       </c>
       <c r="M6" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N6" t="s">
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="2" t="e">
+        <f>K2/SUM(K1:K3)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="P6" s="2">
         <v>100</v>
       </c>
       <c r="T6" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U6" t="s">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" s="2" t="e">
+        <f>R2/SUM(R1:R3)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="W6" s="2">
         <v>100</v>
       </c>
       <c r="AA6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB6" s="2" t="e">
+        <f>Y2/SUM(Y1:Y3)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -1207,40 +1246,40 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G7" t="e">
-        <f>SUM(F1:F3)</f>
+        <f>D3/SUM(D1:D3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I7" s="2">
         <v>100</v>
       </c>
       <c r="M7" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N7" t="e">
-        <f>SUM(M1:M3)</f>
+        <f>K3/SUM(K1:K3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P7" s="2">
         <v>100</v>
       </c>
       <c r="T7" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U7" t="e">
-        <f>SUM(T1:T3)</f>
+        <f>R3/SUM(R1:R3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W7" s="2">
         <v>100</v>
       </c>
       <c r="AA7" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB7" t="e">
-        <f>SUM(AA1:AA3)</f>
+        <f>Y3/SUM(Y1:Y3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1256,21 +1295,21 @@
         <v>100</v>
       </c>
       <c r="M8" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P8" s="2">
         <v>100</v>
       </c>
       <c r="T8" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W8" s="2">
         <v>100</v>
       </c>
       <c r="AA8" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1282,26 +1321,38 @@
         <f>AVERAGEIF(C:C,C9,D:D)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="I9" s="2">
         <v>100</v>
       </c>
       <c r="M9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="P9" s="2">
         <v>100</v>
       </c>
       <c r="T9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="W9" s="2">
         <v>100</v>
       </c>
       <c r="AA9" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
@@ -1312,26 +1363,42 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G10">
+        <f>SUMIF(C:C,C1,D:D)</f>
+        <v>0</v>
+      </c>
       <c r="I10" s="2">
         <v>100</v>
       </c>
       <c r="M10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10">
+        <f>SUMIF(J:J,J1,K:K)</f>
+        <v>0</v>
       </c>
       <c r="P10" s="2">
         <v>100</v>
       </c>
       <c r="T10" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U10">
+        <f>SUMIF(Q:Q,Q1,R:R)</f>
+        <v>0</v>
       </c>
       <c r="W10" s="2">
         <v>100</v>
       </c>
       <c r="AA10" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB10">
+        <f>SUMIF(X:X,X1,Y:Y)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
@@ -1342,26 +1409,38 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="I11" s="2">
         <v>100</v>
       </c>
       <c r="M11" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="P11" s="2">
         <v>100</v>
       </c>
       <c r="T11" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="W11" s="2">
         <v>100</v>
       </c>
       <c r="AA11" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
@@ -1372,25 +1451,41 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G12" t="e">
+        <f>AVERAGEIF(C:C,C2,D:D)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I12" s="2">
         <v>100</v>
       </c>
       <c r="M12" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" t="e">
+        <f>AVERAGEIF(J:J,J2,K:K)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P12" s="2">
         <v>100</v>
       </c>
       <c r="T12" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U12" t="e">
+        <f>AVERAGEIF(Q:Q,Q2,R:R)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W12" s="2">
         <v>100</v>
       </c>
       <c r="AA12" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB12" t="e">
+        <f>AVERAGEIF(X:X,X2,Y:Y)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1402,26 +1497,38 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G13" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="I13" s="2">
         <v>100</v>
       </c>
       <c r="M13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="P13" s="2">
         <v>100</v>
       </c>
       <c r="T13" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="W13" s="2">
         <v>100</v>
       </c>
       <c r="AA13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
@@ -1432,25 +1539,41 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G14" t="e">
+        <f>AVERAGEIF(C:C,C3,D:D)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I14" s="2">
         <v>100</v>
       </c>
       <c r="M14" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N14" t="e">
+        <f>AVERAGEIF(J:J,J3,K:K)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P14" s="2">
         <v>100</v>
       </c>
       <c r="T14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U14" t="e">
+        <f>AVERAGEIF(Q:Q,Q3,R:R)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W14" s="2">
         <v>100</v>
       </c>
       <c r="AA14" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB14" t="e">
+        <f>AVERAGEIF(X:X,X3,Y:Y)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1462,26 +1585,38 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="I15" s="2">
         <v>100</v>
       </c>
       <c r="M15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="P15" s="2">
         <v>100</v>
       </c>
       <c r="T15" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="W15" s="2">
         <v>100</v>
       </c>
       <c r="AA15" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
@@ -1492,29 +1627,45 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G16" t="e">
+        <f>SUM(G10,G12,G14)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I16" s="2">
         <v>100</v>
       </c>
       <c r="M16" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" t="e">
+        <f>SUM(N10,N12,N14)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P16" s="2">
         <v>100</v>
       </c>
       <c r="T16" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U16" t="e">
+        <f>SUM(U10,U12,U14)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W16" s="2">
         <v>100</v>
       </c>
       <c r="AA16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB16" t="e">
+        <f>SUM(AB10,AB12,AB14)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>100</v>
       </c>
@@ -1526,25 +1677,25 @@
         <v>100</v>
       </c>
       <c r="M17" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P17" s="2">
         <v>100</v>
       </c>
       <c r="T17" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W17" s="2">
         <v>100</v>
       </c>
       <c r="AA17" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>100</v>
       </c>
@@ -1556,25 +1707,25 @@
         <v>100</v>
       </c>
       <c r="M18" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P18" s="2">
         <v>100</v>
       </c>
       <c r="T18" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W18" s="2">
         <v>100</v>
       </c>
       <c r="AA18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>100</v>
       </c>
@@ -1586,25 +1737,25 @@
         <v>100</v>
       </c>
       <c r="M19" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P19" s="2">
         <v>100</v>
       </c>
       <c r="T19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W19" s="2">
         <v>100</v>
       </c>
       <c r="AA19" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>100</v>
       </c>
@@ -1612,29 +1763,41 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G20" s="6">
+        <v>100</v>
+      </c>
       <c r="I20" s="2">
         <v>100</v>
       </c>
       <c r="M20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="6">
+        <v>100</v>
       </c>
       <c r="P20" s="2">
         <v>100</v>
       </c>
       <c r="T20" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U20" s="6">
+        <v>100</v>
       </c>
       <c r="W20" s="2">
         <v>100</v>
       </c>
       <c r="AA20" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB20" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>100</v>
       </c>
@@ -1642,29 +1805,45 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G21" t="e">
+        <f>D1/SUM(D1:D3)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I21" s="2">
         <v>100</v>
       </c>
       <c r="M21" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" t="e">
+        <f>K1/SUM(K1:K3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P21" s="2">
         <v>100</v>
       </c>
       <c r="T21" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U21" t="e">
+        <f>R1/SUM(R1:R3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W21" s="2">
         <v>100</v>
       </c>
       <c r="AA21" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB21" t="e">
+        <f>Y1/SUM(Y1:Y3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>100</v>
       </c>
@@ -1672,29 +1851,45 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G22" t="e">
+        <f>D2/SUM(D1:D3)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I22" s="2">
         <v>100</v>
       </c>
       <c r="M22" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" t="e">
+        <f>K2/SUM(K1:K3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P22" s="2">
         <v>100</v>
       </c>
       <c r="T22" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U22" t="e">
+        <f>R2/SUM(R1:R3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W22" s="2">
         <v>100</v>
       </c>
       <c r="AA22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB22" t="e">
+        <f>Y2/SUM(Y1:Y3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>100</v>
       </c>
@@ -1702,29 +1897,45 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G23" t="e">
+        <f>D3/SUM(D1:D3)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I23" s="2">
         <v>100</v>
       </c>
       <c r="M23" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" t="e">
+        <f>K3/SUM(K1:K3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
       </c>
       <c r="T23" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U23" t="e">
+        <f>R3/SUM(R1:R3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W23" s="2">
         <v>100</v>
       </c>
       <c r="AA23" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB23" t="e">
+        <f>Y3/SUM(Y1:Y3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>100</v>
       </c>
@@ -1736,25 +1947,25 @@
         <v>100</v>
       </c>
       <c r="M24" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P24" s="2">
         <v>100</v>
       </c>
       <c r="T24" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W24" s="2">
         <v>100</v>
       </c>
       <c r="AA24" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>100</v>
       </c>
@@ -1762,29 +1973,41 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G25" s="6">
+        <v>200</v>
+      </c>
       <c r="I25" s="2">
         <v>100</v>
       </c>
       <c r="M25" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" s="6">
+        <v>200</v>
       </c>
       <c r="P25" s="2">
         <v>100</v>
       </c>
       <c r="T25" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U25" s="6">
+        <v>200</v>
       </c>
       <c r="W25" s="2">
         <v>100</v>
       </c>
       <c r="AA25" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB25" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <v>100</v>
       </c>
@@ -1792,29 +2015,45 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G26" t="e">
+        <f>D52/SUM(D52:D54)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I26" s="2">
         <v>100</v>
       </c>
       <c r="M26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N26" t="e">
+        <f>K52/SUM(K52:K54)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P26" s="2">
         <v>100</v>
       </c>
       <c r="T26" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U26" t="e">
+        <f>R52/SUM(R52:R54)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W26" s="2">
         <v>100</v>
       </c>
       <c r="AA26" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB26" t="e">
+        <f>Y52/SUM(Y52:Y54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
         <v>100</v>
       </c>
@@ -1822,29 +2061,45 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G27" t="e">
+        <f>D53/SUM(D52:D54)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I27" s="2">
         <v>100</v>
       </c>
       <c r="M27" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N27" t="e">
+        <f>K53/SUM(K52:K54)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P27" s="2">
         <v>100</v>
       </c>
       <c r="T27" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U27" t="e">
+        <f>R53/SUM(R52:R54)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W27" s="2">
         <v>100</v>
       </c>
       <c r="AA27" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB27" t="e">
+        <f>Y53/SUM(Y52:Y54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>100</v>
       </c>
@@ -1852,29 +2107,45 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G28" t="e">
+        <f>D54/SUM(D52:D54)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I28" s="2">
         <v>100</v>
       </c>
       <c r="M28" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N28" t="e">
+        <f>K54/SUM(K52:K54)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P28" s="2">
         <v>100</v>
       </c>
       <c r="T28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U28" t="e">
+        <f>R54/SUM(R52:R54)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W28" s="2">
         <v>100</v>
       </c>
       <c r="AA28" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB28" t="e">
+        <f>Y54/SUM(Y52:Y54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
         <v>100</v>
       </c>
@@ -1886,25 +2157,25 @@
         <v>100</v>
       </c>
       <c r="M29" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P29" s="2">
         <v>100</v>
       </c>
       <c r="T29" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W29" s="2">
         <v>100</v>
       </c>
       <c r="AA29" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
         <v>100</v>
       </c>
@@ -1912,29 +2183,41 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G30" s="6">
+        <v>300</v>
+      </c>
       <c r="I30" s="2">
         <v>100</v>
       </c>
       <c r="M30" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N30" s="6">
+        <v>300</v>
       </c>
       <c r="P30" s="2">
         <v>100</v>
       </c>
       <c r="T30" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U30" s="6">
+        <v>300</v>
       </c>
       <c r="W30" s="2">
         <v>100</v>
       </c>
       <c r="AA30" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB30" s="6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
         <v>100</v>
       </c>
@@ -1942,29 +2225,45 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G31" t="e">
+        <f>D103/SUM(D103:D105)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I31" s="2">
         <v>100</v>
       </c>
       <c r="M31" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N31" t="e">
+        <f>K103/SUM(K103:K105)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P31" s="2">
         <v>100</v>
       </c>
       <c r="T31" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U31" t="e">
+        <f>R103/SUM(R103:R105)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W31" s="2">
         <v>100</v>
       </c>
       <c r="AA31" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB31" t="e">
+        <f>Y103/SUM(Y103:Y105)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>100</v>
       </c>
@@ -1972,651 +2271,923 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G32" t="e">
+        <f>D104/SUM(D103:D105)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I32" s="2">
         <v>100</v>
       </c>
       <c r="M32" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N32" t="e">
+        <f>K104/SUM(K103:K105)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P32" s="2">
         <v>100</v>
       </c>
       <c r="T32" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U32" t="e">
+        <f>R104/SUM(R103:R105)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W32" s="2">
         <v>100</v>
       </c>
       <c r="AA32" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB32" t="e">
+        <f>Y104/SUM(Y103:Y105)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
         <v>100</v>
       </c>
       <c r="F33" t="e">
-        <f t="shared" ref="F33:F51" si="4">AVERAGEIF(C:C,C33,D:D)</f>
+        <f t="shared" ref="F33:F51" si="8">AVERAGEIF(C:C,C33,D:D)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G33" t="e">
+        <f>D105/SUM(D103:D105)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I33" s="2">
         <v>100</v>
       </c>
       <c r="M33" t="e">
-        <f t="shared" ref="M33:M53" si="5">AVERAGEIF(J:J,J33,K:K)</f>
+        <f t="shared" ref="M33:M53" si="9">AVERAGEIF(J:J,J33,K:K)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N33" t="e">
+        <f>K105/SUM(K103:K105)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P33" s="2">
         <v>100</v>
       </c>
       <c r="T33" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U33" t="e">
+        <f>R105/SUM(R103:R105)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W33" s="2">
         <v>100</v>
       </c>
       <c r="AA33" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB33" t="e">
+        <f>Y105/SUM(Y103:Y105)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B34" s="2">
         <v>100</v>
       </c>
       <c r="F34" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="2">
+        <v>100</v>
+      </c>
+      <c r="M34" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P34" s="2">
+        <v>100</v>
+      </c>
+      <c r="T34" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I34" s="2">
-        <v>100</v>
-      </c>
-      <c r="M34" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P34" s="2">
-        <v>100</v>
-      </c>
-      <c r="T34" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W34" s="2">
         <v>100</v>
       </c>
       <c r="AA34" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B35" s="2">
         <v>100</v>
       </c>
       <c r="F35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G35" s="6">
+        <v>400</v>
+      </c>
+      <c r="I35" s="2">
+        <v>100</v>
+      </c>
+      <c r="M35" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N35" s="6">
+        <v>400</v>
+      </c>
+      <c r="P35" s="2">
+        <v>100</v>
+      </c>
+      <c r="T35" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I35" s="2">
-        <v>100</v>
-      </c>
-      <c r="M35" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" s="2">
-        <v>100</v>
-      </c>
-      <c r="T35" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="U35" s="6">
+        <v>400</v>
       </c>
       <c r="W35" s="2">
         <v>100</v>
       </c>
       <c r="AA35" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB35" s="6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B36" s="2">
         <v>100</v>
       </c>
       <c r="F36" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G36" t="e">
+        <f>D154/SUM(D154:D156)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" s="2">
+        <v>100</v>
+      </c>
+      <c r="M36" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N36" t="e">
+        <f>K154/SUM(K154:K156)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P36" s="2">
+        <v>100</v>
+      </c>
+      <c r="T36" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I36" s="2">
-        <v>100</v>
-      </c>
-      <c r="M36" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P36" s="2">
-        <v>100</v>
-      </c>
-      <c r="T36" t="e">
-        <f t="shared" si="3"/>
+      <c r="U36" t="e">
+        <f>R154/SUM(R154:R156)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W36" s="2">
         <v>100</v>
       </c>
       <c r="AA36" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB36" t="e">
+        <f>Y154/SUM(Y154:Y156)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B37" s="2">
         <v>100</v>
       </c>
       <c r="F37" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G37" t="e">
+        <f>D155/SUM(D154:D156)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="2">
+        <v>100</v>
+      </c>
+      <c r="M37" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N37" t="e">
+        <f>K155/SUM(K154:K156)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P37" s="2">
+        <v>100</v>
+      </c>
+      <c r="T37" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I37" s="2">
-        <v>100</v>
-      </c>
-      <c r="M37" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P37" s="2">
-        <v>100</v>
-      </c>
-      <c r="T37" t="e">
-        <f t="shared" si="3"/>
+      <c r="U37" t="e">
+        <f>R155/SUM(R154:R156)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W37" s="2">
         <v>100</v>
       </c>
       <c r="AA37" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB37" t="e">
+        <f>Y155/SUM(Y154:Y156)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
         <v>100</v>
       </c>
       <c r="F38" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G38" t="e">
+        <f>D156/SUM(D154:D156)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="2">
+        <v>100</v>
+      </c>
+      <c r="M38" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N38" t="e">
+        <f>K156/SUM(K154:K156)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P38" s="2">
+        <v>100</v>
+      </c>
+      <c r="T38" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I38" s="2">
-        <v>100</v>
-      </c>
-      <c r="M38" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P38" s="2">
-        <v>100</v>
-      </c>
-      <c r="T38" t="e">
-        <f t="shared" si="3"/>
+      <c r="U38" t="e">
+        <f>R156/SUM(R154:R156)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W38" s="2">
         <v>100</v>
       </c>
       <c r="AA38" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB38" t="e">
+        <f>Y156/SUM(Y154:Y156)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
         <v>100</v>
       </c>
       <c r="F39" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" s="2">
+        <v>100</v>
+      </c>
+      <c r="M39" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P39" s="2">
+        <v>100</v>
+      </c>
+      <c r="T39" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I39" s="2">
-        <v>100</v>
-      </c>
-      <c r="M39" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P39" s="2">
-        <v>100</v>
-      </c>
-      <c r="T39" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W39" s="2">
         <v>100</v>
       </c>
       <c r="AA39" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
         <v>100</v>
       </c>
       <c r="F40" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G40" s="6">
+        <v>500</v>
+      </c>
+      <c r="I40" s="2">
+        <v>100</v>
+      </c>
+      <c r="M40" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N40" s="6">
+        <v>500</v>
+      </c>
+      <c r="P40" s="2">
+        <v>100</v>
+      </c>
+      <c r="T40" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I40" s="2">
-        <v>100</v>
-      </c>
-      <c r="M40" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P40" s="2">
-        <v>100</v>
-      </c>
-      <c r="T40" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="U40" s="6">
+        <v>500</v>
       </c>
       <c r="W40" s="2">
         <v>100</v>
       </c>
       <c r="AA40" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB40" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
         <v>100</v>
       </c>
       <c r="F41" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G41" t="e">
+        <f>D205/SUM(D205:D207)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" s="2">
+        <v>100</v>
+      </c>
+      <c r="M41" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N41" t="e">
+        <f>K205/SUM(K205:K207)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P41" s="2">
+        <v>100</v>
+      </c>
+      <c r="T41" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I41" s="2">
-        <v>100</v>
-      </c>
-      <c r="M41" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P41" s="2">
-        <v>100</v>
-      </c>
-      <c r="T41" t="e">
-        <f t="shared" si="3"/>
+      <c r="U41" t="e">
+        <f>R205/SUM(R205:R207)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W41" s="2">
         <v>100</v>
       </c>
       <c r="AA41" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB41" t="e">
+        <f>Y205/SUM(Y205:Y207)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B42" s="2">
         <v>100</v>
       </c>
       <c r="F42" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G42" t="e">
+        <f>D206/SUM(D205:D207)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" s="2">
+        <v>100</v>
+      </c>
+      <c r="M42" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N42" t="e">
+        <f>K206/SUM(K205:K207)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P42" s="2">
+        <v>100</v>
+      </c>
+      <c r="T42" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I42" s="2">
-        <v>100</v>
-      </c>
-      <c r="M42" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P42" s="2">
-        <v>100</v>
-      </c>
-      <c r="T42" t="e">
-        <f t="shared" si="3"/>
+      <c r="U42" t="e">
+        <f>R206/SUM(R205:R207)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W42" s="2">
         <v>100</v>
       </c>
       <c r="AA42" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB42" t="e">
+        <f>Y206/SUM(Y205:Y207)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B43" s="2">
         <v>100</v>
       </c>
       <c r="F43" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G43" t="e">
+        <f>D207/SUM(D205:D207)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" s="2">
+        <v>100</v>
+      </c>
+      <c r="M43" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N43" t="e">
+        <f>K207/SUM(K205:K207)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P43" s="2">
+        <v>100</v>
+      </c>
+      <c r="T43" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I43" s="2">
-        <v>100</v>
-      </c>
-      <c r="M43" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P43" s="2">
-        <v>100</v>
-      </c>
-      <c r="T43" t="e">
-        <f t="shared" si="3"/>
+      <c r="U43" t="e">
+        <f>R207/SUM(R205:R207)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W43" s="2">
         <v>100</v>
       </c>
       <c r="AA43" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB43" t="e">
+        <f>Y207/SUM(Y205:Y207)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B44" s="2">
         <v>100</v>
       </c>
       <c r="F44" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I44" s="2">
+        <v>100</v>
+      </c>
+      <c r="M44" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P44" s="2">
+        <v>100</v>
+      </c>
+      <c r="T44" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I44" s="2">
-        <v>100</v>
-      </c>
-      <c r="M44" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P44" s="2">
-        <v>100</v>
-      </c>
-      <c r="T44" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W44" s="2">
         <v>100</v>
       </c>
       <c r="AA44" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B45" s="2">
         <v>100</v>
       </c>
       <c r="F45" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G45" s="6">
+        <v>600</v>
+      </c>
+      <c r="I45" s="2">
+        <v>100</v>
+      </c>
+      <c r="M45" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N45" s="6">
+        <v>600</v>
+      </c>
+      <c r="P45" s="2">
+        <v>100</v>
+      </c>
+      <c r="T45" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I45" s="2">
-        <v>100</v>
-      </c>
-      <c r="M45" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P45" s="2">
-        <v>100</v>
-      </c>
-      <c r="T45" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="U45" s="6">
+        <v>600</v>
       </c>
       <c r="W45" s="2">
         <v>100</v>
       </c>
       <c r="AA45" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB45" s="6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="46" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B46" s="2">
         <v>100</v>
       </c>
       <c r="F46" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" t="e">
+        <f>D256/SUM(D256:D258)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" s="2">
+        <v>100</v>
+      </c>
+      <c r="M46" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N46" t="e">
+        <f>K256/SUM(K256:K258)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P46" s="2">
+        <v>100</v>
+      </c>
+      <c r="T46" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I46" s="2">
-        <v>100</v>
-      </c>
-      <c r="M46" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P46" s="2">
-        <v>100</v>
-      </c>
-      <c r="T46" t="e">
-        <f t="shared" si="3"/>
+      <c r="U46" t="e">
+        <f>R256/SUM(R256:R258)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W46" s="2">
         <v>100</v>
       </c>
       <c r="AA46" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB46" t="e">
+        <f>Y256/SUM(Y256:Y258)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B47" s="2">
         <v>100</v>
       </c>
       <c r="F47" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" t="e">
+        <f>D257/SUM(D256:D258)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I47" s="2">
+        <v>100</v>
+      </c>
+      <c r="M47" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N47" t="e">
+        <f>K257/SUM(K256:K258)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P47" s="2">
+        <v>100</v>
+      </c>
+      <c r="T47" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I47" s="2">
-        <v>100</v>
-      </c>
-      <c r="M47" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P47" s="2">
-        <v>100</v>
-      </c>
-      <c r="T47" t="e">
-        <f t="shared" si="3"/>
+      <c r="U47" t="e">
+        <f>R257/SUM(R256:R258)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W47" s="2">
         <v>100</v>
       </c>
       <c r="AA47" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB47" t="e">
+        <f>Y257/SUM(Y256:Y258)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B48" s="2">
         <v>100</v>
       </c>
       <c r="F48" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G48" t="e">
+        <f>D258/SUM(D256:D258)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I48" s="2">
+        <v>100</v>
+      </c>
+      <c r="M48" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N48" t="e">
+        <f>K258/SUM(K256:K258)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P48" s="2">
+        <v>100</v>
+      </c>
+      <c r="T48" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I48" s="2">
-        <v>100</v>
-      </c>
-      <c r="M48" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P48" s="2">
-        <v>100</v>
-      </c>
-      <c r="T48" t="e">
-        <f t="shared" si="3"/>
+      <c r="U48" t="e">
+        <f>R258/SUM(R256:R258)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W48" s="2">
         <v>100</v>
       </c>
       <c r="AA48" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="49" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB48" t="e">
+        <f>Y258/SUM(Y256:Y258)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B49" s="2">
         <v>100</v>
       </c>
       <c r="F49" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I49" s="2">
+        <v>100</v>
+      </c>
+      <c r="M49" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P49" s="2">
+        <v>100</v>
+      </c>
+      <c r="T49" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I49" s="2">
-        <v>100</v>
-      </c>
-      <c r="M49" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P49" s="2">
-        <v>100</v>
-      </c>
-      <c r="T49" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W49" s="2">
         <v>100</v>
       </c>
       <c r="AA49" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
         <v>100</v>
       </c>
       <c r="F50" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G50" s="6">
+        <v>700</v>
+      </c>
+      <c r="I50" s="2">
+        <v>100</v>
+      </c>
+      <c r="M50" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N50" s="6">
+        <v>700</v>
+      </c>
+      <c r="P50" s="2">
+        <v>100</v>
+      </c>
+      <c r="T50" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I50" s="2">
-        <v>100</v>
-      </c>
-      <c r="M50" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P50" s="2">
-        <v>100</v>
-      </c>
-      <c r="T50" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="U50" s="6">
+        <v>700</v>
       </c>
       <c r="W50" s="2">
         <v>100</v>
       </c>
       <c r="AA50" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="51" spans="2:27" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB50" s="6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="51" spans="2:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
         <v>100</v>
       </c>
       <c r="F51" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G51" t="e">
+        <f>D307/SUM(D307:D309)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I51" s="2">
+        <v>100</v>
+      </c>
+      <c r="M51" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N51" t="e">
+        <f>K307/SUM(K307:K309)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P51" s="2">
+        <v>100</v>
+      </c>
+      <c r="T51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I51" s="2">
-        <v>100</v>
-      </c>
-      <c r="M51" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P51" s="2">
-        <v>100</v>
-      </c>
-      <c r="T51" t="e">
-        <f t="shared" si="3"/>
+      <c r="U51" t="e">
+        <f>R307/SUM(R307:R309)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W51" s="2">
         <v>100</v>
       </c>
       <c r="AA51" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB51" t="e">
+        <f>Y307/SUM(Y307:Y309)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B52" s="2">
         <v>200</v>
       </c>
+      <c r="G52" t="e">
+        <f>D308/SUM(D307:D309)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I52" s="2">
         <v>200</v>
       </c>
       <c r="M52" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N52" t="e">
+        <f>K308/SUM(K307:K309)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P52" s="2">
         <v>200</v>
       </c>
       <c r="T52" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U52" t="e">
+        <f>R308/SUM(R307:R309)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W52" s="2">
         <v>200</v>
       </c>
       <c r="AA52" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB52" t="e">
+        <f>Y308/SUM(Y307:Y309)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B53" s="2">
         <v>200</v>
       </c>
+      <c r="G53" t="e">
+        <f>D309/SUM(D307:D309)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I53" s="2">
         <v>200</v>
       </c>
       <c r="M53" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N53" t="e">
+        <f>K309/SUM(K307:K309)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P53" s="2">
         <v>200</v>
       </c>
       <c r="T53" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U53" t="e">
+        <f>R309/SUM(R307:R309)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W53" s="2">
         <v>200</v>
       </c>
       <c r="AA53" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB53" t="e">
+        <f>Y309/SUM(Y307:Y309)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B54" s="2">
         <v>200</v>
       </c>
@@ -2630,63 +3201,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B55" s="2">
         <v>200</v>
       </c>
+      <c r="G55" s="6">
+        <v>800</v>
+      </c>
       <c r="I55" s="2">
         <v>200</v>
       </c>
+      <c r="N55" s="6">
+        <v>800</v>
+      </c>
       <c r="P55" s="2">
         <v>200</v>
       </c>
+      <c r="U55" s="6">
+        <v>800</v>
+      </c>
       <c r="W55" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB55" s="6">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="56" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B56" s="2">
         <v>200</v>
       </c>
+      <c r="G56" t="e">
+        <f>D358/SUM(D358:D360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I56" s="2">
         <v>200</v>
       </c>
+      <c r="N56" t="e">
+        <f>K358/SUM(K358:K360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P56" s="2">
         <v>200</v>
       </c>
+      <c r="U56" t="e">
+        <f>R358/SUM(R358:R360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W56" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="57" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB56" t="e">
+        <f>Y358/SUM(Y358:Y360)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B57" s="2">
         <v>200</v>
       </c>
+      <c r="G57" t="e">
+        <f>D359/SUM(D358:D360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I57" s="2">
         <v>200</v>
       </c>
+      <c r="N57" t="e">
+        <f>K359/SUM(K358:K360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P57" s="2">
         <v>200</v>
       </c>
+      <c r="U57" t="e">
+        <f>R359/SUM(R358:R360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W57" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="58" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB57" t="e">
+        <f>Y359/SUM(Y358:Y360)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B58" s="2">
         <v>200</v>
       </c>
+      <c r="G58" t="e">
+        <f>D360/SUM(D358:D360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I58" s="2">
         <v>200</v>
       </c>
+      <c r="N58" t="e">
+        <f>K360/SUM(K358:K360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P58" s="2">
         <v>200</v>
       </c>
+      <c r="U58" t="e">
+        <f>R360/SUM(R358:R360)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W58" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="59" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB58" t="e">
+        <f>Y360/SUM(Y358:Y360)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B59" s="2">
         <v>200</v>
       </c>
@@ -2700,63 +3331,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="60" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B60" s="2">
         <v>200</v>
       </c>
+      <c r="G60" s="6">
+        <v>900</v>
+      </c>
       <c r="I60" s="2">
         <v>200</v>
       </c>
+      <c r="N60" s="6">
+        <v>900</v>
+      </c>
       <c r="P60" s="2">
         <v>200</v>
       </c>
+      <c r="U60" s="6">
+        <v>900</v>
+      </c>
       <c r="W60" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="61" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB60" s="6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="61" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B61" s="2">
         <v>200</v>
       </c>
+      <c r="G61" t="e">
+        <f>D409/SUM(D409:D411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I61" s="2">
         <v>200</v>
       </c>
+      <c r="N61" t="e">
+        <f>K409/SUM(K409:K411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P61" s="2">
         <v>200</v>
       </c>
+      <c r="U61" t="e">
+        <f>R409/SUM(R409:R411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W61" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="62" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB61" t="e">
+        <f>Y409/SUM(Y409:Y411)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B62" s="2">
         <v>200</v>
       </c>
+      <c r="G62" t="e">
+        <f>D410/SUM(D409:D411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I62" s="2">
         <v>200</v>
       </c>
+      <c r="N62" t="e">
+        <f>K410/SUM(K409:K411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P62" s="2">
         <v>200</v>
       </c>
+      <c r="U62" t="e">
+        <f>R410/SUM(R409:R411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W62" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="63" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB62" t="e">
+        <f>Y410/SUM(Y409:Y411)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B63" s="2">
         <v>200</v>
       </c>
+      <c r="G63" t="e">
+        <f>D411/SUM(D409:D411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I63" s="2">
         <v>200</v>
       </c>
+      <c r="N63" t="e">
+        <f>K411/SUM(K409:K411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P63" s="2">
         <v>200</v>
       </c>
+      <c r="U63" t="e">
+        <f>R411/SUM(R409:R411)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W63" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="64" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB63" t="e">
+        <f>Y411/SUM(Y409:Y411)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B64" s="2">
         <v>200</v>
       </c>
@@ -2770,63 +3461,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B65" s="2">
         <v>200</v>
       </c>
+      <c r="G65" s="6">
+        <v>1000</v>
+      </c>
       <c r="I65" s="2">
         <v>200</v>
       </c>
+      <c r="N65" s="6">
+        <v>1000</v>
+      </c>
       <c r="P65" s="2">
         <v>200</v>
       </c>
+      <c r="U65" s="6">
+        <v>1000</v>
+      </c>
       <c r="W65" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="66" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB65" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="66" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B66" s="2">
         <v>200</v>
       </c>
+      <c r="G66" t="e">
+        <f>D460/SUM(D460:D462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I66" s="2">
         <v>200</v>
       </c>
+      <c r="N66" t="e">
+        <f>K460/SUM(K460:K462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P66" s="2">
         <v>200</v>
       </c>
+      <c r="U66" t="e">
+        <f>R460/SUM(R460:R462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W66" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="67" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB66" t="e">
+        <f>Y460/SUM(Y460:Y462)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B67" s="2">
         <v>200</v>
       </c>
+      <c r="G67" t="e">
+        <f>D461/SUM(D460:D462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I67" s="2">
         <v>200</v>
       </c>
+      <c r="N67" t="e">
+        <f>K461/SUM(K460:K462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P67" s="2">
         <v>200</v>
       </c>
+      <c r="U67" t="e">
+        <f>R461/SUM(R460:R462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W67" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="68" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB67" t="e">
+        <f>Y461/SUM(Y460:Y462)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B68" s="2">
         <v>200</v>
       </c>
+      <c r="G68" t="e">
+        <f>D462/SUM(D460:D462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I68" s="2">
         <v>200</v>
       </c>
+      <c r="N68" t="e">
+        <f>K462/SUM(K460:K462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P68" s="2">
         <v>200</v>
       </c>
+      <c r="U68" t="e">
+        <f>R462/SUM(R460:R462)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W68" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="69" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB68" t="e">
+        <f>Y462/SUM(Y460:Y462)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B69" s="2">
         <v>200</v>
       </c>
@@ -2840,63 +3591,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B70" s="2">
         <v>200</v>
       </c>
+      <c r="G70" s="6">
+        <v>1100</v>
+      </c>
       <c r="I70" s="2">
         <v>200</v>
       </c>
+      <c r="N70" s="6">
+        <v>1100</v>
+      </c>
       <c r="P70" s="2">
         <v>200</v>
       </c>
+      <c r="U70" s="6">
+        <v>1100</v>
+      </c>
       <c r="W70" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="71" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB70" s="6">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="71" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B71" s="2">
         <v>200</v>
       </c>
+      <c r="G71" t="e">
+        <f>D511/SUM(D511:D513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I71" s="2">
         <v>200</v>
       </c>
+      <c r="N71" t="e">
+        <f>K511/SUM(K511:K513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P71" s="2">
         <v>200</v>
       </c>
+      <c r="U71" t="e">
+        <f>R511/SUM(R511:R513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W71" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="72" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB71" t="e">
+        <f>Y511/SUM(Y511:Y513)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B72" s="2">
         <v>200</v>
       </c>
+      <c r="G72" t="e">
+        <f>D512/SUM(D511:D513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I72" s="2">
         <v>200</v>
       </c>
+      <c r="N72" t="e">
+        <f>K512/SUM(K511:K513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P72" s="2">
         <v>200</v>
       </c>
+      <c r="U72" t="e">
+        <f>R512/SUM(R511:R513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W72" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="73" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB72" t="e">
+        <f>Y512/SUM(Y511:Y513)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B73" s="2">
         <v>200</v>
       </c>
+      <c r="G73" t="e">
+        <f>D513/SUM(D511:D513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I73" s="2">
         <v>200</v>
       </c>
+      <c r="N73" t="e">
+        <f>K513/SUM(K511:K513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P73" s="2">
         <v>200</v>
       </c>
+      <c r="U73" t="e">
+        <f>R513/SUM(R511:R513)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W73" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="74" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB73" t="e">
+        <f>Y513/SUM(Y511:Y513)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B74" s="2">
         <v>200</v>
       </c>
@@ -2910,63 +3721,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="75" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B75" s="2">
         <v>200</v>
       </c>
+      <c r="G75" s="6">
+        <v>1200</v>
+      </c>
       <c r="I75" s="2">
         <v>200</v>
       </c>
+      <c r="N75" s="6">
+        <v>1200</v>
+      </c>
       <c r="P75" s="2">
         <v>200</v>
       </c>
+      <c r="U75" s="6">
+        <v>1200</v>
+      </c>
       <c r="W75" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="76" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB75" s="6">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="76" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B76" s="2">
         <v>200</v>
       </c>
+      <c r="G76" t="e">
+        <f>D562/SUM(D562:D564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I76" s="2">
         <v>200</v>
       </c>
+      <c r="N76" t="e">
+        <f>K562/SUM(K562:K564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P76" s="2">
         <v>200</v>
       </c>
+      <c r="U76" t="e">
+        <f>R562/SUM(R562:R564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W76" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="77" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB76" t="e">
+        <f>Y562/SUM(Y562:Y564)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B77" s="2">
         <v>200</v>
       </c>
+      <c r="G77" t="e">
+        <f>D563/SUM(D562:D564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I77" s="2">
         <v>200</v>
       </c>
+      <c r="N77" t="e">
+        <f>K563/SUM(K562:K564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P77" s="2">
         <v>200</v>
       </c>
+      <c r="U77" t="e">
+        <f>R563/SUM(R562:R564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W77" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="78" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB77" t="e">
+        <f>Y563/SUM(Y562:Y564)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B78" s="2">
         <v>200</v>
       </c>
+      <c r="G78" t="e">
+        <f>D564/SUM(D562:D564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I78" s="2">
         <v>200</v>
       </c>
+      <c r="N78" t="e">
+        <f>K564/SUM(K562:K564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P78" s="2">
         <v>200</v>
       </c>
+      <c r="U78" t="e">
+        <f>R564/SUM(R562:R564)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W78" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="79" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB78" t="e">
+        <f>Y564/SUM(Y562:Y564)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B79" s="2">
         <v>200</v>
       </c>
@@ -2980,63 +3851,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="80" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B80" s="2">
         <v>200</v>
       </c>
+      <c r="G80" s="6">
+        <v>1300</v>
+      </c>
       <c r="I80" s="2">
         <v>200</v>
       </c>
+      <c r="N80" s="6">
+        <v>1300</v>
+      </c>
       <c r="P80" s="2">
         <v>200</v>
       </c>
+      <c r="U80" s="6">
+        <v>1300</v>
+      </c>
       <c r="W80" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="81" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB80" s="6">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="81" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B81" s="2">
         <v>200</v>
       </c>
+      <c r="G81" t="e">
+        <f>D613/SUM(D613:D615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I81" s="2">
         <v>200</v>
       </c>
+      <c r="N81" t="e">
+        <f>K613/SUM(K613:K615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P81" s="2">
         <v>200</v>
       </c>
+      <c r="U81" t="e">
+        <f>R613/SUM(R613:R615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W81" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="82" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB81" t="e">
+        <f>Y613/SUM(Y613:Y615)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B82" s="2">
         <v>200</v>
       </c>
+      <c r="G82" t="e">
+        <f>D614/SUM(D613:D615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I82" s="2">
         <v>200</v>
       </c>
+      <c r="N82" t="e">
+        <f>K614/SUM(K613:K615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P82" s="2">
         <v>200</v>
       </c>
+      <c r="U82" t="e">
+        <f>R614/SUM(R613:R615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W82" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="83" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB82" t="e">
+        <f>Y614/SUM(Y613:Y615)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B83" s="2">
         <v>200</v>
       </c>
+      <c r="G83" t="e">
+        <f>D615/SUM(D613:D615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I83" s="2">
         <v>200</v>
       </c>
+      <c r="N83" t="e">
+        <f>K615/SUM(K613:K615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P83" s="2">
         <v>200</v>
       </c>
+      <c r="U83" t="e">
+        <f>R615/SUM(R613:R615)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W83" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="84" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB83" t="e">
+        <f>Y615/SUM(Y613:Y615)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B84" s="2">
         <v>200</v>
       </c>
@@ -3050,63 +3981,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B85" s="2">
         <v>200</v>
       </c>
+      <c r="G85" s="6">
+        <v>1400</v>
+      </c>
       <c r="I85" s="2">
         <v>200</v>
       </c>
+      <c r="N85" s="6">
+        <v>1400</v>
+      </c>
       <c r="P85" s="2">
         <v>200</v>
       </c>
+      <c r="U85" s="6">
+        <v>1400</v>
+      </c>
       <c r="W85" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="86" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB85" s="6">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="86" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B86" s="2">
         <v>200</v>
       </c>
+      <c r="G86" t="e">
+        <f>D664/SUM(D664:D666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I86" s="2">
         <v>200</v>
       </c>
+      <c r="N86" t="e">
+        <f>K664/SUM(K664:K666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P86" s="2">
         <v>200</v>
       </c>
+      <c r="U86" t="e">
+        <f>R664/SUM(R664:R666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W86" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="87" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB86" t="e">
+        <f>Y664/SUM(Y664:Y666)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B87" s="2">
         <v>200</v>
       </c>
+      <c r="G87" t="e">
+        <f>D665/SUM(D664:D666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I87" s="2">
         <v>200</v>
       </c>
+      <c r="N87" t="e">
+        <f>K665/SUM(K664:K666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P87" s="2">
         <v>200</v>
       </c>
+      <c r="U87" t="e">
+        <f>R665/SUM(R664:R666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W87" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="88" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB87" t="e">
+        <f>Y665/SUM(Y664:Y666)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B88" s="2">
         <v>200</v>
       </c>
+      <c r="G88" t="e">
+        <f>D666/SUM(D664:D666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I88" s="2">
         <v>200</v>
       </c>
+      <c r="N88" t="e">
+        <f>K666/SUM(K664:K666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P88" s="2">
         <v>200</v>
       </c>
+      <c r="U88" t="e">
+        <f>R666/SUM(R664:R666)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W88" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="89" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB88" t="e">
+        <f>Y666/SUM(Y664:Y666)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B89" s="2">
         <v>200</v>
       </c>
@@ -3120,63 +4111,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="90" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B90" s="2">
         <v>200</v>
       </c>
+      <c r="G90" s="6">
+        <v>1500</v>
+      </c>
       <c r="I90" s="2">
         <v>200</v>
       </c>
+      <c r="N90" s="6">
+        <v>1500</v>
+      </c>
       <c r="P90" s="2">
         <v>200</v>
       </c>
+      <c r="U90" s="6">
+        <v>1500</v>
+      </c>
       <c r="W90" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="91" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB90" s="6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="91" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B91" s="2">
         <v>200</v>
       </c>
+      <c r="G91" t="e">
+        <f>D715/SUM(D715:D717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I91" s="2">
         <v>200</v>
       </c>
+      <c r="N91" t="e">
+        <f>K715/SUM(K715:K717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P91" s="2">
         <v>200</v>
       </c>
+      <c r="U91" t="e">
+        <f>R715/SUM(R715:R717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W91" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="92" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB91" t="e">
+        <f>Y715/SUM(Y715:Y717)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B92" s="2">
         <v>200</v>
       </c>
+      <c r="G92" t="e">
+        <f>D716/SUM(D715:D717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I92" s="2">
         <v>200</v>
       </c>
+      <c r="N92" t="e">
+        <f>K716/SUM(K715:K717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P92" s="2">
         <v>200</v>
       </c>
+      <c r="U92" t="e">
+        <f>R716/SUM(R715:R717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W92" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="93" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB92" t="e">
+        <f>Y716/SUM(Y715:Y717)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B93" s="2">
         <v>200</v>
       </c>
+      <c r="G93" t="e">
+        <f>D717/SUM(D715:D717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I93" s="2">
         <v>200</v>
       </c>
+      <c r="N93" t="e">
+        <f>K717/SUM(K715:K717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P93" s="2">
         <v>200</v>
       </c>
+      <c r="U93" t="e">
+        <f>R717/SUM(R715:R717)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W93" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="94" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB93" t="e">
+        <f>Y717/SUM(Y715:Y717)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B94" s="2">
         <v>200</v>
       </c>
@@ -3190,63 +4241,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B95" s="2">
         <v>200</v>
       </c>
+      <c r="G95" s="6">
+        <v>1600</v>
+      </c>
       <c r="I95" s="2">
         <v>200</v>
       </c>
+      <c r="N95" s="6">
+        <v>1600</v>
+      </c>
       <c r="P95" s="2">
         <v>200</v>
       </c>
+      <c r="U95" s="6">
+        <v>1600</v>
+      </c>
       <c r="W95" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="96" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB95" s="6">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="96" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B96" s="2">
         <v>200</v>
       </c>
+      <c r="G96" t="e">
+        <f>D766/SUM(D766:D768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I96" s="2">
         <v>200</v>
       </c>
+      <c r="N96" t="e">
+        <f>K766/SUM(K766:K768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P96" s="2">
         <v>200</v>
       </c>
+      <c r="U96" t="e">
+        <f>R766/SUM(R766:R768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W96" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="97" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB96" t="e">
+        <f>Y766/SUM(Y766:Y768)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B97" s="2">
         <v>200</v>
       </c>
+      <c r="G97" t="e">
+        <f>D767/SUM(D766:D768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I97" s="2">
         <v>200</v>
       </c>
+      <c r="N97" t="e">
+        <f>K767/SUM(K766:K768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P97" s="2">
         <v>200</v>
       </c>
+      <c r="U97" t="e">
+        <f>R767/SUM(R766:R768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W97" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB97" t="e">
+        <f>Y767/SUM(Y766:Y768)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B98" s="2">
         <v>200</v>
       </c>
+      <c r="G98" t="e">
+        <f>D768/SUM(D766:D768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I98" s="2">
         <v>200</v>
       </c>
+      <c r="N98" t="e">
+        <f>K768/SUM(K766:K768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P98" s="2">
         <v>200</v>
       </c>
+      <c r="U98" t="e">
+        <f>R768/SUM(R766:R768)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W98" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="99" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB98" t="e">
+        <f>Y768/SUM(Y766:Y768)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B99" s="2">
         <v>200</v>
       </c>
@@ -3260,63 +4371,123 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B100" s="2">
         <v>200</v>
       </c>
+      <c r="G100" s="6">
+        <v>1700</v>
+      </c>
       <c r="I100" s="2">
         <v>200</v>
       </c>
+      <c r="N100" s="6">
+        <v>1700</v>
+      </c>
       <c r="P100" s="2">
         <v>200</v>
       </c>
+      <c r="U100" s="6">
+        <v>1700</v>
+      </c>
       <c r="W100" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="101" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB100" s="6">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="101" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B101" s="2">
         <v>200</v>
       </c>
+      <c r="G101" t="e">
+        <f>D827/SUM(D827:D829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I101" s="2">
         <v>200</v>
       </c>
+      <c r="N101" t="e">
+        <f>K827/SUM(K827:K829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P101" s="2">
         <v>200</v>
       </c>
+      <c r="U101" t="e">
+        <f>R827/SUM(R827:R829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W101" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="102" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB101" t="e">
+        <f>Y827/SUM(Y827:Y829)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B102" s="2">
         <v>200</v>
       </c>
+      <c r="G102" t="e">
+        <f>D828/SUM(D827:D829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I102" s="2">
         <v>200</v>
       </c>
+      <c r="N102" t="e">
+        <f>K828/SUM(K827:K829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P102" s="2">
         <v>200</v>
       </c>
+      <c r="U102" t="e">
+        <f>R828/SUM(R827:R829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W102" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="103" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB102" t="e">
+        <f>Y828/SUM(Y827:Y829)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="103" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B103" s="2">
         <v>300</v>
       </c>
+      <c r="G103" t="e">
+        <f>D829/SUM(D827:D829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I103" s="2">
         <v>300</v>
       </c>
+      <c r="N103" t="e">
+        <f>K829/SUM(K827:K829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P103" s="2">
         <v>300</v>
       </c>
+      <c r="U103" t="e">
+        <f>R829/SUM(R827:R829)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W103" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="104" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB103" t="e">
+        <f>Y829/SUM(Y827:Y829)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="104" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B104" s="2">
         <v>300</v>
       </c>
@@ -3330,63 +4501,123 @@
         <v>300</v>
       </c>
     </row>
-    <row r="105" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B105" s="2">
         <v>300</v>
       </c>
+      <c r="G105" s="6">
+        <v>1800</v>
+      </c>
       <c r="I105" s="2">
         <v>300</v>
       </c>
+      <c r="N105" s="6">
+        <v>1800</v>
+      </c>
       <c r="P105" s="2">
         <v>300</v>
       </c>
+      <c r="U105" s="6">
+        <v>1800</v>
+      </c>
       <c r="W105" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="106" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB105" s="6">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="106" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B106" s="2">
         <v>300</v>
       </c>
+      <c r="G106" t="e">
+        <f>D878/SUM(D878:D880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I106" s="2">
         <v>300</v>
       </c>
+      <c r="N106" t="e">
+        <f>K878/SUM(K878:K880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P106" s="2">
         <v>300</v>
       </c>
+      <c r="U106" t="e">
+        <f>R878/SUM(R878:R880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W106" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="107" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB106" t="e">
+        <f>Y878/SUM(Y878:Y880)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="107" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B107" s="2">
         <v>300</v>
       </c>
+      <c r="G107" t="e">
+        <f>D879/SUM(D878:D880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I107" s="2">
         <v>300</v>
       </c>
+      <c r="N107" t="e">
+        <f>K879/SUM(K878:K880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P107" s="2">
         <v>300</v>
       </c>
+      <c r="U107" t="e">
+        <f>R879/SUM(R878:R880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W107" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="108" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB107" t="e">
+        <f>Y879/SUM(Y878:Y880)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="108" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B108" s="2">
         <v>300</v>
       </c>
+      <c r="G108" t="e">
+        <f>D880/SUM(D878:D880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I108" s="2">
         <v>300</v>
       </c>
+      <c r="N108" t="e">
+        <f>K880/SUM(K878:K880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P108" s="2">
         <v>300</v>
       </c>
+      <c r="U108" t="e">
+        <f>R880/SUM(R878:R880)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W108" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="109" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="AB108" t="e">
+        <f>Y880/SUM(Y878:Y880)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="109" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B109" s="2">
         <v>300</v>
       </c>
@@ -3400,7 +4631,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="110" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B110" s="2">
         <v>300</v>
       </c>
@@ -3414,7 +4645,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="111" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B111" s="2">
         <v>300</v>
       </c>
@@ -3428,7 +4659,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="112" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B112" s="2">
         <v>300</v>
       </c>

</xml_diff>

<commit_message>
organized the default and weaker models in weka folder
</commit_message>
<xml_diff>
--- a/scripts/drone_app/processLogs/Comparison_template.xlsx
+++ b/scripts/drone_app/processLogs/Comparison_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasamanamannejad/workspace_all/research/edge-offloading/sim_results/ite1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasamanamannejad/workspace_all/research/edge-offloading/sim_results/ite4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84265A2C-99E5-2F4A-B29B-B4CFABD7852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF41013-5407-1C46-8EE6-7A46C7CF4F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="26860" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="600" windowWidth="27800" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL_APP" sheetId="9" r:id="rId1"/>
@@ -934,21 +934,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEDCC7C-376D-924C-AAF9-C175A48D41DA}">
   <dimension ref="A1:AB969"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Y1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="4.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="18.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="4.1640625" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" customWidth="1"/>
     <col min="9" max="9" width="5.1640625" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="5"/>
+    <col min="10" max="10" width="7.6640625" style="5" customWidth="1"/>
     <col min="11" max="11" width="7.1640625" style="5" customWidth="1"/>
     <col min="12" max="12" width="4.1640625" customWidth="1"/>
     <col min="14" max="14" width="15.5" customWidth="1"/>
@@ -1032,40 +1032,40 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G2" t="e">
-        <f t="shared" ref="G2:G3" si="1">AVERAGE(G22,G27,G32,G37,G42,G47,G52,G57,G62,G67,G72,G77,G82,G87,G92,G97,G102,G107)</f>
+        <f>AVERAGE(G22,G27,G32,G37,G42,G47,G52,G57,G62,G67,G72,G77,G82,G87,G92,G97,G102,G107)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I2" s="2">
         <v>100</v>
       </c>
       <c r="M2" t="e">
-        <f t="shared" ref="M2:M32" si="2">AVERAGEIF(J:J,J2,K:K)</f>
+        <f t="shared" ref="M2:M32" si="1">AVERAGEIF(J:J,J2,K:K)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N2" t="e">
-        <f t="shared" ref="N2:N3" si="3">AVERAGE(N22,N27,N32,N37,N42,N47,N52,N57,N62,N67,N72,N77,N82,N87,N92,N97,N102,N107)</f>
+        <f>AVERAGE(N22,N27,N32,N37,N42,N47,N52,N57,N62,N67,N72,N77,N82,N87,N92,N97,N102,N107)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P2" s="2">
         <v>100</v>
       </c>
       <c r="T2" t="e">
-        <f t="shared" ref="T2:T53" si="4">AVERAGEIF(Q:Q,Q2,R:R)</f>
+        <f t="shared" ref="T2:T53" si="2">AVERAGEIF(Q:Q,Q2,R:R)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U2" t="e">
-        <f t="shared" ref="U2:U3" si="5">AVERAGE(U22,U27,U32,U37,U42,U47,U52,U57,U62,U67,U72,U77,U82,U87,U92,U97,U102,U107)</f>
+        <f>AVERAGE(U22,U27,U32,U37,U42,U47,U52,U57,U62,U67,U72,U77,U82,U87,U92,U97,U102,U107)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W2" s="2">
         <v>100</v>
       </c>
       <c r="AA2" t="e">
-        <f t="shared" ref="AA2:AA53" si="6">AVERAGEIF(X:X,X2,Y:Y)</f>
+        <f t="shared" ref="AA2:AA53" si="3">AVERAGEIF(X:X,X2,Y:Y)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB2" t="e">
-        <f t="shared" ref="AB2:AB3" si="7">AVERAGE(AB22,AB27,AB32,AB37,AB42,AB47,AB52,AB57,AB62,AB67,AB72,AB77,AB82,AB87,AB92,AB97,AB102,AB107)</f>
+        <f>AVERAGE(AB22,AB27,AB32,AB37,AB42,AB47,AB52,AB57,AB62,AB67,AB72,AB77,AB82,AB87,AB92,AB97,AB102,AB107)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1078,40 +1078,40 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G3" t="e">
+        <f t="shared" ref="G3" si="4">AVERAGE(G23,G28,G33,G38,G43,G48,G53,G58,G63,G68,G73,G78,G83,G88,G93,G98,G103,G108)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" s="2">
+        <v>100</v>
+      </c>
+      <c r="M3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I3" s="2">
-        <v>100</v>
-      </c>
-      <c r="M3" t="e">
+      <c r="N3" t="e">
+        <f t="shared" ref="N3" si="5">AVERAGE(N23,N28,N33,N38,N43,N48,N53,N58,N63,N68,N73,N78,N83,N88,N93,N98,N103,N108)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P3" s="2">
+        <v>100</v>
+      </c>
+      <c r="T3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N3" t="e">
+      <c r="U3" t="e">
+        <f t="shared" ref="U3" si="6">AVERAGE(U23,U28,U33,U38,U43,U48,U53,U58,U63,U68,U73,U78,U83,U88,U93,U98,U103,U108)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W3" s="2">
+        <v>100</v>
+      </c>
+      <c r="AA3" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P3" s="2">
-        <v>100</v>
-      </c>
-      <c r="T3" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U3" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W3" s="2">
-        <v>100</v>
-      </c>
-      <c r="AA3" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="AB3" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AB3" si="7">AVERAGE(AB23,AB28,AB33,AB38,AB43,AB48,AB53,AB58,AB63,AB68,AB73,AB78,AB83,AB88,AB93,AB98,AB103,AB108)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1134,18 +1134,18 @@
         <v>100</v>
       </c>
       <c r="T4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W4" s="2">
         <v>100</v>
       </c>
       <c r="AA4" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>100</v>
       </c>
@@ -1154,40 +1154,40 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G5" t="e">
-        <f>D1/SUM(D1:D3)</f>
+        <f>F1/SUM(F1:F3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I5" s="2">
         <v>100</v>
       </c>
       <c r="M5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" t="e">
+        <f>M1/SUM(M1:M3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="2">
+        <v>100</v>
+      </c>
+      <c r="T5" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N5" t="e">
-        <f>K1/SUM(K1:K3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="2">
-        <v>100</v>
-      </c>
-      <c r="T5" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="U5" t="e">
-        <f>R1/SUM(R1:R3)</f>
+        <f>T1/SUM(T1:T3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W5" s="2">
         <v>100</v>
       </c>
       <c r="AA5" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB5" t="e">
-        <f>Y1/SUM(Y1:Y3)</f>
+        <f>AA1/SUM(AA1:AA3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1200,40 +1200,40 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G6" s="2" t="e">
-        <f>D2/SUM(D1:D3)</f>
+        <f>F2/SUM(F1:F3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I6" s="2">
         <v>100</v>
       </c>
       <c r="M6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="2" t="e">
+        <f>M2/SUM(M1:M3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="2">
+        <v>100</v>
+      </c>
+      <c r="T6" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="2" t="e">
-        <f>K2/SUM(K1:K3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="2">
-        <v>100</v>
-      </c>
-      <c r="T6" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="U6" s="2" t="e">
-        <f>R2/SUM(R1:R3)</f>
+        <f>T2/SUM(T1:T3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W6" s="2">
         <v>100</v>
       </c>
       <c r="AA6" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB6" s="2" t="e">
-        <f>Y2/SUM(Y1:Y3)</f>
+        <f>AA2/SUM(AA1:AA3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1246,40 +1246,40 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G7" t="e">
-        <f>D3/SUM(D1:D3)</f>
+        <f>F3/SUM(F1:F3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I7" s="2">
         <v>100</v>
       </c>
       <c r="M7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" t="e">
+        <f>M3/SUM(M1:M3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="2">
+        <v>100</v>
+      </c>
+      <c r="T7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N7" t="e">
-        <f>K3/SUM(K1:K3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="2">
-        <v>100</v>
-      </c>
-      <c r="T7" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="U7" t="e">
-        <f>R3/SUM(R1:R3)</f>
+        <f>T3/SUM(T1:T3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W7" s="2">
         <v>100</v>
       </c>
       <c r="AA7" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB7" t="e">
-        <f>Y3/SUM(Y1:Y3)</f>
+        <f>AA3/SUM(AA1:AA3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1295,21 +1295,21 @@
         <v>100</v>
       </c>
       <c r="M8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="2">
+        <v>100</v>
+      </c>
+      <c r="T8" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P8" s="2">
-        <v>100</v>
-      </c>
-      <c r="T8" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W8" s="2">
         <v>100</v>
       </c>
       <c r="AA8" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1328,7 +1328,7 @@
         <v>100</v>
       </c>
       <c r="M9" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N9" s="2" t="s">
@@ -1338,7 +1338,7 @@
         <v>100</v>
       </c>
       <c r="T9" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U9" s="2" t="s">
@@ -1348,7 +1348,7 @@
         <v>100</v>
       </c>
       <c r="AA9" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB9" s="2" t="s">
@@ -1371,7 +1371,7 @@
         <v>100</v>
       </c>
       <c r="M10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N10">
@@ -1382,7 +1382,7 @@
         <v>100</v>
       </c>
       <c r="T10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U10">
@@ -1393,7 +1393,7 @@
         <v>100</v>
       </c>
       <c r="AA10" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB10">
@@ -1416,7 +1416,7 @@
         <v>100</v>
       </c>
       <c r="M11" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N11" s="2" t="s">
@@ -1426,7 +1426,7 @@
         <v>100</v>
       </c>
       <c r="T11" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U11" s="2" t="s">
@@ -1436,7 +1436,7 @@
         <v>100</v>
       </c>
       <c r="AA11" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB11" s="2" t="s">
@@ -1459,7 +1459,7 @@
         <v>100</v>
       </c>
       <c r="M12" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N12" t="e">
@@ -1470,7 +1470,7 @@
         <v>100</v>
       </c>
       <c r="T12" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U12" t="e">
@@ -1481,7 +1481,7 @@
         <v>100</v>
       </c>
       <c r="AA12" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB12" t="e">
@@ -1504,7 +1504,7 @@
         <v>100</v>
       </c>
       <c r="M13" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N13" s="2" t="s">
@@ -1514,7 +1514,7 @@
         <v>100</v>
       </c>
       <c r="T13" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U13" s="2" t="s">
@@ -1524,7 +1524,7 @@
         <v>100</v>
       </c>
       <c r="AA13" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB13" s="2" t="s">
@@ -1547,7 +1547,7 @@
         <v>100</v>
       </c>
       <c r="M14" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N14" t="e">
@@ -1558,7 +1558,7 @@
         <v>100</v>
       </c>
       <c r="T14" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U14" t="e">
@@ -1569,7 +1569,7 @@
         <v>100</v>
       </c>
       <c r="AA14" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB14" t="e">
@@ -1592,7 +1592,7 @@
         <v>100</v>
       </c>
       <c r="M15" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N15" s="2" t="s">
@@ -1602,7 +1602,7 @@
         <v>100</v>
       </c>
       <c r="T15" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U15" s="2" t="s">
@@ -1612,7 +1612,7 @@
         <v>100</v>
       </c>
       <c r="AA15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB15" s="2" t="s">
@@ -1635,7 +1635,7 @@
         <v>100</v>
       </c>
       <c r="M16" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N16" t="e">
@@ -1646,7 +1646,7 @@
         <v>100</v>
       </c>
       <c r="T16" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U16" t="e">
@@ -1657,7 +1657,7 @@
         <v>100</v>
       </c>
       <c r="AA16" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB16" t="e">
@@ -1673,25 +1673,41 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="G17" t="e">
+        <f>G10/G16</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="I17" s="2">
         <v>100</v>
       </c>
       <c r="M17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" t="e">
+        <f>N10/N16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="2">
+        <v>100</v>
+      </c>
+      <c r="T17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P17" s="2">
-        <v>100</v>
-      </c>
-      <c r="T17" t="e">
-        <f t="shared" si="4"/>
+      <c r="U17" t="e">
+        <f>U10/U16</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W17" s="2">
         <v>100</v>
       </c>
       <c r="AA17" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB17" t="e">
+        <f>AB10/AB16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1707,21 +1723,21 @@
         <v>100</v>
       </c>
       <c r="M18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="2">
+        <v>100</v>
+      </c>
+      <c r="T18" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P18" s="2">
-        <v>100</v>
-      </c>
-      <c r="T18" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W18" s="2">
         <v>100</v>
       </c>
       <c r="AA18" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1737,21 +1753,21 @@
         <v>100</v>
       </c>
       <c r="M19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="2">
+        <v>100</v>
+      </c>
+      <c r="T19" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P19" s="2">
-        <v>100</v>
-      </c>
-      <c r="T19" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W19" s="2">
         <v>100</v>
       </c>
       <c r="AA19" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1770,19 +1786,19 @@
         <v>100</v>
       </c>
       <c r="M20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="6">
+        <v>100</v>
+      </c>
+      <c r="P20" s="2">
+        <v>100</v>
+      </c>
+      <c r="T20" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N20" s="6">
-        <v>100</v>
-      </c>
-      <c r="P20" s="2">
-        <v>100</v>
-      </c>
-      <c r="T20" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="U20" s="6">
         <v>100</v>
       </c>
@@ -1790,7 +1806,7 @@
         <v>100</v>
       </c>
       <c r="AA20" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="6">
@@ -1813,7 +1829,7 @@
         <v>100</v>
       </c>
       <c r="M21" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N21" t="e">
@@ -1824,7 +1840,7 @@
         <v>100</v>
       </c>
       <c r="T21" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U21" t="e">
@@ -1835,7 +1851,7 @@
         <v>100</v>
       </c>
       <c r="AA21" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB21" t="e">
@@ -1859,7 +1875,7 @@
         <v>100</v>
       </c>
       <c r="M22" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N22" t="e">
@@ -1870,7 +1886,7 @@
         <v>100</v>
       </c>
       <c r="T22" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U22" t="e">
@@ -1881,7 +1897,7 @@
         <v>100</v>
       </c>
       <c r="AA22" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB22" t="e">
@@ -1905,7 +1921,7 @@
         <v>100</v>
       </c>
       <c r="M23" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N23" t="e">
@@ -1916,7 +1932,7 @@
         <v>100</v>
       </c>
       <c r="T23" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U23" t="e">
@@ -1927,7 +1943,7 @@
         <v>100</v>
       </c>
       <c r="AA23" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB23" t="e">
@@ -1947,21 +1963,21 @@
         <v>100</v>
       </c>
       <c r="M24" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P24" s="2">
+        <v>100</v>
+      </c>
+      <c r="T24" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P24" s="2">
-        <v>100</v>
-      </c>
-      <c r="T24" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W24" s="2">
         <v>100</v>
       </c>
       <c r="AA24" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1980,19 +1996,19 @@
         <v>100</v>
       </c>
       <c r="M25" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" s="6">
+        <v>200</v>
+      </c>
+      <c r="P25" s="2">
+        <v>100</v>
+      </c>
+      <c r="T25" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N25" s="6">
-        <v>200</v>
-      </c>
-      <c r="P25" s="2">
-        <v>100</v>
-      </c>
-      <c r="T25" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="U25" s="6">
         <v>200</v>
       </c>
@@ -2000,7 +2016,7 @@
         <v>100</v>
       </c>
       <c r="AA25" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB25" s="6">
@@ -2023,7 +2039,7 @@
         <v>100</v>
       </c>
       <c r="M26" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N26" t="e">
@@ -2034,7 +2050,7 @@
         <v>100</v>
       </c>
       <c r="T26" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U26" t="e">
@@ -2045,7 +2061,7 @@
         <v>100</v>
       </c>
       <c r="AA26" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB26" t="e">
@@ -2069,7 +2085,7 @@
         <v>100</v>
       </c>
       <c r="M27" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N27" t="e">
@@ -2080,7 +2096,7 @@
         <v>100</v>
       </c>
       <c r="T27" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U27" t="e">
@@ -2091,7 +2107,7 @@
         <v>100</v>
       </c>
       <c r="AA27" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB27" t="e">
@@ -2115,7 +2131,7 @@
         <v>100</v>
       </c>
       <c r="M28" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N28" t="e">
@@ -2126,7 +2142,7 @@
         <v>100</v>
       </c>
       <c r="T28" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U28" t="e">
@@ -2137,7 +2153,7 @@
         <v>100</v>
       </c>
       <c r="AA28" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB28" t="e">
@@ -2157,21 +2173,21 @@
         <v>100</v>
       </c>
       <c r="M29" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P29" s="2">
+        <v>100</v>
+      </c>
+      <c r="T29" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P29" s="2">
-        <v>100</v>
-      </c>
-      <c r="T29" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="W29" s="2">
         <v>100</v>
       </c>
       <c r="AA29" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2190,19 +2206,19 @@
         <v>100</v>
       </c>
       <c r="M30" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N30" s="6">
+        <v>300</v>
+      </c>
+      <c r="P30" s="2">
+        <v>100</v>
+      </c>
+      <c r="T30" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N30" s="6">
-        <v>300</v>
-      </c>
-      <c r="P30" s="2">
-        <v>100</v>
-      </c>
-      <c r="T30" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="U30" s="6">
         <v>300</v>
       </c>
@@ -2210,7 +2226,7 @@
         <v>100</v>
       </c>
       <c r="AA30" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB30" s="6">
@@ -2233,7 +2249,7 @@
         <v>100</v>
       </c>
       <c r="M31" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N31" t="e">
@@ -2244,7 +2260,7 @@
         <v>100</v>
       </c>
       <c r="T31" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U31" t="e">
@@ -2255,7 +2271,7 @@
         <v>100</v>
       </c>
       <c r="AA31" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB31" t="e">
@@ -2279,7 +2295,7 @@
         <v>100</v>
       </c>
       <c r="M32" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N32" t="e">
@@ -2290,7 +2306,7 @@
         <v>100</v>
       </c>
       <c r="T32" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U32" t="e">
@@ -2301,7 +2317,7 @@
         <v>100</v>
       </c>
       <c r="AA32" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB32" t="e">
@@ -2336,7 +2352,7 @@
         <v>100</v>
       </c>
       <c r="T33" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U33" t="e">
@@ -2347,7 +2363,7 @@
         <v>100</v>
       </c>
       <c r="AA33" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB33" t="e">
@@ -2374,14 +2390,14 @@
         <v>100</v>
       </c>
       <c r="T34" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W34" s="2">
         <v>100</v>
       </c>
       <c r="AA34" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2410,7 +2426,7 @@
         <v>100</v>
       </c>
       <c r="T35" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U35" s="6">
@@ -2420,7 +2436,7 @@
         <v>100</v>
       </c>
       <c r="AA35" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB35" s="6">
@@ -2454,7 +2470,7 @@
         <v>100</v>
       </c>
       <c r="T36" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U36" t="e">
@@ -2465,7 +2481,7 @@
         <v>100</v>
       </c>
       <c r="AA36" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB36" t="e">
@@ -2500,7 +2516,7 @@
         <v>100</v>
       </c>
       <c r="T37" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U37" t="e">
@@ -2511,7 +2527,7 @@
         <v>100</v>
       </c>
       <c r="AA37" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB37" t="e">
@@ -2546,7 +2562,7 @@
         <v>100</v>
       </c>
       <c r="T38" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U38" t="e">
@@ -2557,7 +2573,7 @@
         <v>100</v>
       </c>
       <c r="AA38" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB38" t="e">
@@ -2584,14 +2600,14 @@
         <v>100</v>
       </c>
       <c r="T39" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W39" s="2">
         <v>100</v>
       </c>
       <c r="AA39" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2620,7 +2636,7 @@
         <v>100</v>
       </c>
       <c r="T40" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U40" s="6">
@@ -2630,7 +2646,7 @@
         <v>100</v>
       </c>
       <c r="AA40" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB40" s="6">
@@ -2664,7 +2680,7 @@
         <v>100</v>
       </c>
       <c r="T41" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U41" t="e">
@@ -2675,7 +2691,7 @@
         <v>100</v>
       </c>
       <c r="AA41" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB41" t="e">
@@ -2710,7 +2726,7 @@
         <v>100</v>
       </c>
       <c r="T42" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U42" t="e">
@@ -2721,7 +2737,7 @@
         <v>100</v>
       </c>
       <c r="AA42" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB42" t="e">
@@ -2756,7 +2772,7 @@
         <v>100</v>
       </c>
       <c r="T43" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U43" t="e">
@@ -2767,7 +2783,7 @@
         <v>100</v>
       </c>
       <c r="AA43" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB43" t="e">
@@ -2794,14 +2810,14 @@
         <v>100</v>
       </c>
       <c r="T44" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W44" s="2">
         <v>100</v>
       </c>
       <c r="AA44" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2830,7 +2846,7 @@
         <v>100</v>
       </c>
       <c r="T45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U45" s="6">
@@ -2840,7 +2856,7 @@
         <v>100</v>
       </c>
       <c r="AA45" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB45" s="6">
@@ -2874,7 +2890,7 @@
         <v>100</v>
       </c>
       <c r="T46" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U46" t="e">
@@ -2885,7 +2901,7 @@
         <v>100</v>
       </c>
       <c r="AA46" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB46" t="e">
@@ -2920,7 +2936,7 @@
         <v>100</v>
       </c>
       <c r="T47" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U47" t="e">
@@ -2931,7 +2947,7 @@
         <v>100</v>
       </c>
       <c r="AA47" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB47" t="e">
@@ -2966,7 +2982,7 @@
         <v>100</v>
       </c>
       <c r="T48" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U48" t="e">
@@ -2977,7 +2993,7 @@
         <v>100</v>
       </c>
       <c r="AA48" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB48" t="e">
@@ -3004,14 +3020,14 @@
         <v>100</v>
       </c>
       <c r="T49" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W49" s="2">
         <v>100</v>
       </c>
       <c r="AA49" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3040,7 +3056,7 @@
         <v>100</v>
       </c>
       <c r="T50" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U50" s="6">
@@ -3050,7 +3066,7 @@
         <v>100</v>
       </c>
       <c r="AA50" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB50" s="6">
@@ -3084,7 +3100,7 @@
         <v>100</v>
       </c>
       <c r="T51" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U51" t="e">
@@ -3095,7 +3111,7 @@
         <v>100</v>
       </c>
       <c r="AA51" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB51" t="e">
@@ -3126,7 +3142,7 @@
         <v>200</v>
       </c>
       <c r="T52" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U52" t="e">
@@ -3137,7 +3153,7 @@
         <v>200</v>
       </c>
       <c r="AA52" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB52" t="e">
@@ -3168,7 +3184,7 @@
         <v>200</v>
       </c>
       <c r="T53" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="U53" t="e">
@@ -3179,7 +3195,7 @@
         <v>200</v>
       </c>
       <c r="AA53" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB53" t="e">
@@ -4402,28 +4418,28 @@
         <v>200</v>
       </c>
       <c r="G101" t="e">
-        <f>D827/SUM(D827:D829)</f>
+        <f>D817/SUM(D817:D819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I101" s="2">
         <v>200</v>
       </c>
       <c r="N101" t="e">
-        <f>K827/SUM(K827:K829)</f>
+        <f>K817/SUM(K817:K819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P101" s="2">
         <v>200</v>
       </c>
       <c r="U101" t="e">
-        <f>R827/SUM(R827:R829)</f>
+        <f>R817/SUM(R817:R819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W101" s="2">
         <v>200</v>
       </c>
       <c r="AB101" t="e">
-        <f>Y827/SUM(Y827:Y829)</f>
+        <f>Y817/SUM(Y817:Y819)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4432,28 +4448,28 @@
         <v>200</v>
       </c>
       <c r="G102" t="e">
-        <f>D828/SUM(D827:D829)</f>
+        <f>D818/SUM(D817:D819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I102" s="2">
         <v>200</v>
       </c>
       <c r="N102" t="e">
-        <f>K828/SUM(K827:K829)</f>
+        <f>K818/SUM(K817:K819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P102" s="2">
         <v>200</v>
       </c>
       <c r="U102" t="e">
-        <f>R828/SUM(R827:R829)</f>
+        <f>R818/SUM(R817:R819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W102" s="2">
         <v>200</v>
       </c>
       <c r="AB102" t="e">
-        <f>Y828/SUM(Y827:Y829)</f>
+        <f>Y818/SUM(Y817:Y819)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4462,28 +4478,28 @@
         <v>300</v>
       </c>
       <c r="G103" t="e">
-        <f>D829/SUM(D827:D829)</f>
+        <f>D819/SUM(D817:D819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I103" s="2">
         <v>300</v>
       </c>
       <c r="N103" t="e">
-        <f>K829/SUM(K827:K829)</f>
+        <f>K819/SUM(K817:K819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P103" s="2">
         <v>300</v>
       </c>
       <c r="U103" t="e">
-        <f>R829/SUM(R827:R829)</f>
+        <f>R819/SUM(R817:R819)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W103" s="2">
         <v>300</v>
       </c>
       <c r="AB103" t="e">
-        <f>Y829/SUM(Y827:Y829)</f>
+        <f>Y819/SUM(Y817:Y819)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4532,28 +4548,28 @@
         <v>300</v>
       </c>
       <c r="G106" t="e">
-        <f>D878/SUM(D878:D880)</f>
+        <f>D868/SUM(D868:D870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I106" s="2">
         <v>300</v>
       </c>
       <c r="N106" t="e">
-        <f>K878/SUM(K878:K880)</f>
+        <f>K868/SUM(K868:K870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P106" s="2">
         <v>300</v>
       </c>
       <c r="U106" t="e">
-        <f>R878/SUM(R878:R880)</f>
+        <f>R868/SUM(R868:R870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W106" s="2">
         <v>300</v>
       </c>
       <c r="AB106" t="e">
-        <f>Y878/SUM(Y878:Y880)</f>
+        <f>Y868/SUM(Y868:Y870)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4562,28 +4578,28 @@
         <v>300</v>
       </c>
       <c r="G107" t="e">
-        <f>D879/SUM(D878:D880)</f>
+        <f>D869/SUM(D868:D870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I107" s="2">
         <v>300</v>
       </c>
       <c r="N107" t="e">
-        <f>K879/SUM(K878:K880)</f>
+        <f>K869/SUM(K868:K870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P107" s="2">
         <v>300</v>
       </c>
       <c r="U107" t="e">
-        <f>R879/SUM(R878:R880)</f>
+        <f>R869/SUM(R868:R870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W107" s="2">
         <v>300</v>
       </c>
       <c r="AB107" t="e">
-        <f>Y879/SUM(Y878:Y880)</f>
+        <f>Y869/SUM(Y868:Y870)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4592,28 +4608,28 @@
         <v>300</v>
       </c>
       <c r="G108" t="e">
-        <f>D880/SUM(D878:D880)</f>
+        <f>D870/SUM(D868:D870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I108" s="2">
         <v>300</v>
       </c>
       <c r="N108" t="e">
-        <f>K880/SUM(K878:K880)</f>
+        <f>K870/SUM(K868:K870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P108" s="2">
         <v>300</v>
       </c>
       <c r="U108" t="e">
-        <f>R880/SUM(R878:R880)</f>
+        <f>R870/SUM(R868:R870)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W108" s="2">
         <v>300</v>
       </c>
       <c r="AB108" t="e">
-        <f>Y880/SUM(Y878:Y880)</f>
+        <f>Y870/SUM(Y868:Y870)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7739,7 +7755,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="332" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="332" spans="2:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B332" s="4">
         <v>700</v>
       </c>

</xml_diff>